<commit_message>
fixed bugs and wrong excel formatting
</commit_message>
<xml_diff>
--- a/datas/courses_desc.xlsx
+++ b/datas/courses_desc.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\important\interesting python projects\zoom_reminder\datas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\important\interesting python projects\zoom_reminder\Class-reminder\datas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E07020FC-9F0D-4F0C-9DAB-AA920442A4F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16A51A25-B2DC-4F74-A066-B153D91D337E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>L10</t>
   </si>
@@ -51,9 +51,6 @@
     <t>V4</t>
   </si>
   <si>
-    <t>Tin 5</t>
-  </si>
-  <si>
     <t>CN3</t>
   </si>
   <si>
@@ -166,6 +163,12 @@
   </si>
   <si>
     <t>Đ1</t>
+  </si>
+  <si>
+    <t>QP2</t>
+  </si>
+  <si>
+    <t>Tin5</t>
   </si>
 </sst>
 </file>
@@ -490,7 +493,7 @@
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -501,27 +504,27 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>12</v>
-      </c>
-      <c r="E1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>0</v>
@@ -535,10 +538,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>1</v>
@@ -547,15 +550,15 @@
         <v>8258073057</v>
       </c>
       <c r="E3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>7</v>
@@ -569,13 +572,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D5">
         <v>6822045197</v>
@@ -586,10 +589,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>2</v>
@@ -603,10 +606,10 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>3</v>
@@ -620,13 +623,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D8">
         <v>7361311308</v>
@@ -637,10 +640,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>5</v>
@@ -649,15 +652,15 @@
         <v>5841603699</v>
       </c>
       <c r="E9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>6</v>
@@ -671,10 +674,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>4</v>
@@ -683,18 +686,18 @@
         <v>7666693318</v>
       </c>
       <c r="E11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D12">
         <v>5678955431</v>
@@ -705,30 +708,30 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>9</v>
+        <v>46</v>
       </c>
       <c r="D13">
         <v>9102597428</v>
       </c>
       <c r="E13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>8</v>
+        <v>47</v>
       </c>
       <c r="D14">
         <v>2066767262</v>

</xml_diff>